<commit_message>
updated vehicles and courses
</commit_message>
<xml_diff>
--- a/Fahrzeug_und_Bedarfsplan.xlsx
+++ b/Fahrzeug_und_Bedarfsplan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
   <si>
     <t>Fahrzeugplanung</t>
   </si>
@@ -188,6 +188,24 @@
   </si>
   <si>
     <t>WLF-Pers. erhält GW-Dekon Lehrgang</t>
+  </si>
+  <si>
+    <t>GruKw</t>
+  </si>
+  <si>
+    <t>leBefKw</t>
+  </si>
+  <si>
+    <t>FüKw</t>
+  </si>
+  <si>
+    <t>GefKw</t>
+  </si>
+  <si>
+    <t>KdoW-LNA</t>
+  </si>
+  <si>
+    <t>KdoW-OrGl</t>
   </si>
 </sst>
 </file>
@@ -622,7 +640,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1248,13 +1266,13 @@
         <v>17</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>35</v>
@@ -1266,12 +1284,14 @@
         <v>35</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q12" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
@@ -1319,12 +1339,14 @@
         <v>2</v>
       </c>
       <c r="O13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P13" s="4">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>1</v>
+      </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
@@ -1483,20 +1505,48 @@
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
@@ -1508,19 +1558,45 @@
     <row r="20" spans="1:23">
       <c r="A20" s="12"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="C20" s="4">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4">
+        <v>9</v>
+      </c>
+      <c r="E20" s="4">
+        <v>9</v>
+      </c>
+      <c r="F20" s="4">
+        <v>9</v>
+      </c>
+      <c r="G20" s="4">
+        <v>9</v>
+      </c>
+      <c r="H20" s="4">
+        <v>9</v>
+      </c>
+      <c r="I20" s="4">
+        <v>9</v>
+      </c>
+      <c r="J20" s="4">
+        <v>9</v>
+      </c>
+      <c r="K20" s="4">
+        <v>9</v>
+      </c>
+      <c r="L20" s="4">
+        <v>3</v>
+      </c>
+      <c r="M20" s="4">
+        <v>3</v>
+      </c>
+      <c r="N20" s="4">
+        <v>3</v>
+      </c>
+      <c r="O20" s="4">
+        <v>3</v>
+      </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -1879,7 +1955,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4">
         <f>SUM(C13:R13)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
@@ -1986,8 +2062,12 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="J37" s="4">
+        <v>9</v>
+      </c>
+      <c r="K37" s="4">
+        <v>3</v>
+      </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -1996,7 +2076,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4">
         <f>SUM(C20:R20)</f>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>

</xml_diff>

<commit_message>
updates (containing LNA / OrgL) and some bugfixes
</commit_message>
<xml_diff>
--- a/Fahrzeug_und_Bedarfsplan.xlsx
+++ b/Fahrzeug_und_Bedarfsplan.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuerwehrgebäude" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171026"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="91">
   <si>
     <t>Fahrzeugplanung</t>
   </si>
@@ -49,63 +50,69 @@
     <t>GW - A</t>
   </si>
   <si>
+    <t>GW-Mes</t>
+  </si>
+  <si>
     <t>SW</t>
   </si>
   <si>
     <t>DLAK</t>
   </si>
   <si>
+    <t>ELW</t>
+  </si>
+  <si>
+    <t>ELW 2</t>
+  </si>
+  <si>
     <t>WLF</t>
   </si>
   <si>
+    <t>RTW</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Öl</t>
+  </si>
+  <si>
+    <t>Hauptwache Nebenstelle</t>
+  </si>
+  <si>
+    <t>GW - H</t>
+  </si>
+  <si>
+    <t>GW - Öl</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>Rüst</t>
+  </si>
+  <si>
+    <t>Löschgruppe</t>
+  </si>
+  <si>
+    <t>Dekon-Wache</t>
+  </si>
+  <si>
     <t>MTW</t>
   </si>
   <si>
-    <t>ELW</t>
-  </si>
-  <si>
-    <t>ELW 2</t>
-  </si>
-  <si>
-    <t>RTW</t>
-  </si>
-  <si>
-    <t>Hauptwache Nebenstelle</t>
-  </si>
-  <si>
-    <t>GW - H</t>
-  </si>
-  <si>
-    <t>RW</t>
-  </si>
-  <si>
-    <t>Rüst</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Öl</t>
-  </si>
-  <si>
-    <t>Löschgruppe</t>
-  </si>
-  <si>
-    <t>Dekon-Wache</t>
-  </si>
-  <si>
     <t>GW - G</t>
   </si>
   <si>
+    <t>GW-G</t>
+  </si>
+  <si>
     <t>GW - Dekon</t>
   </si>
   <si>
     <t>GW - Mess</t>
   </si>
   <si>
-    <t>GW - Öl</t>
-  </si>
-  <si>
     <t>ÖL</t>
   </si>
   <si>
@@ -124,6 +131,12 @@
     <t>NEF</t>
   </si>
   <si>
+    <t>KdoW-LNA</t>
+  </si>
+  <si>
+    <t>KdoW-OrGl</t>
+  </si>
+  <si>
     <t>Helipad</t>
   </si>
   <si>
@@ -142,6 +155,18 @@
     <t>BePo</t>
   </si>
   <si>
+    <t>GruKw</t>
+  </si>
+  <si>
+    <t>leBefKw</t>
+  </si>
+  <si>
+    <t>FüKw</t>
+  </si>
+  <si>
+    <t>GefKw</t>
+  </si>
+  <si>
     <t>THW</t>
   </si>
   <si>
@@ -157,9 +182,6 @@
     <t>GW-Mess</t>
   </si>
   <si>
-    <t>GW-G</t>
-  </si>
-  <si>
     <t>GW-Dekon</t>
   </si>
   <si>
@@ -169,6 +191,12 @@
     <t>Notarzt</t>
   </si>
   <si>
+    <t>LNA</t>
+  </si>
+  <si>
+    <t>OrgL</t>
+  </si>
+  <si>
     <t>ZF leBefKw</t>
   </si>
   <si>
@@ -190,28 +218,82 @@
     <t>WLF-Pers. erhält GW-Dekon Lehrgang</t>
   </si>
   <si>
-    <t>GruKw</t>
-  </si>
-  <si>
-    <t>leBefKw</t>
-  </si>
-  <si>
-    <t>FüKw</t>
-  </si>
-  <si>
-    <t>GefKw</t>
-  </si>
-  <si>
-    <t>KdoW-LNA</t>
-  </si>
-  <si>
-    <t>KdoW-OrGl</t>
+    <t>Feuerwachen</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>Ort</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>Fahrzeuge</t>
+  </si>
+  <si>
+    <t>Info / Notiz</t>
+  </si>
+  <si>
+    <t>Spenge</t>
+  </si>
+  <si>
+    <t>Spenge-Mitte (Altbau)</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>Spenge-Mitte (Neubau)</t>
+  </si>
+  <si>
+    <t>Bünde</t>
+  </si>
+  <si>
+    <t>Hauptwache Bünde</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>Hauptwache Bünde (Nebengebäude)</t>
+  </si>
+  <si>
+    <t>HWN</t>
+  </si>
+  <si>
+    <t>Löhne</t>
+  </si>
+  <si>
+    <t>Porta Westfalica</t>
+  </si>
+  <si>
+    <t>Barkenhausen</t>
+  </si>
+  <si>
+    <t>Bad Oeynhausen</t>
+  </si>
+  <si>
+    <t>Oberbecksen</t>
+  </si>
+  <si>
+    <t>Minden</t>
+  </si>
+  <si>
+    <t>Hauptwache Minden</t>
+  </si>
+  <si>
+    <t>Hauptwache Minden (Nebengebäude)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -282,16 +364,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -304,6 +383,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -320,7 +402,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -629,21 +715,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="18" width="11.7109375" customWidth="1"/>
@@ -758,29 +844,31 @@
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="J3" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>15</v>
@@ -799,8 +887,12 @@
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
+      <c r="U3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="W3" s="4"/>
     </row>
     <row r="4" spans="1:23">
@@ -819,12 +911,14 @@
         <v>9</v>
       </c>
       <c r="G4" s="4">
-        <v>9</v>
-      </c>
-      <c r="H4" s="4">
-        <v>3</v>
-      </c>
-      <c r="I4" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="H4" s="7">
+        <v>3</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3</v>
+      </c>
       <c r="J4" s="4">
         <v>3</v>
       </c>
@@ -832,19 +926,19 @@
         <v>3</v>
       </c>
       <c r="L4" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M4" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N4" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O4" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P4" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="4">
         <v>2</v>
@@ -861,7 +955,7 @@
     <row r="5" spans="1:23">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -870,54 +964,54 @@
         <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="16"/>
       <c r="O5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="W5" s="4"/>
     </row>
@@ -937,31 +1031,31 @@
         <v>9</v>
       </c>
       <c r="G6" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H6" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I6" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J6" s="4">
         <v>3</v>
       </c>
       <c r="K6" s="4">
-        <v>9</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8">
-        <v>3</v>
-      </c>
-      <c r="N6" s="4">
-        <v>3</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L6" s="4">
+        <v>9</v>
+      </c>
+      <c r="M6" s="7">
+        <v>9</v>
+      </c>
+      <c r="N6" s="16"/>
       <c r="O6" s="4">
         <v>3</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="7">
         <v>3</v>
       </c>
       <c r="Q6" s="4">
@@ -979,7 +1073,7 @@
     <row r="7" spans="1:23">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -997,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>9</v>
@@ -1009,17 +1103,17 @@
         <v>9</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="N7" s="6"/>
       <c r="O7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="Q7" s="4" t="s">
         <v>17</v>
@@ -1029,13 +1123,13 @@
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="W7" s="4"/>
     </row>
@@ -1075,7 +1169,7 @@
       <c r="M8" s="4">
         <v>3</v>
       </c>
-      <c r="N8" s="7"/>
+      <c r="N8" s="6"/>
       <c r="O8" s="4">
         <v>3</v>
       </c>
@@ -1097,7 +1191,7 @@
     <row r="9" spans="1:23">
       <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -1109,54 +1203,54 @@
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="H9" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -1190,13 +1284,13 @@
         <v>3</v>
       </c>
       <c r="L10" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M10" s="4">
         <v>6</v>
       </c>
       <c r="N10" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O10" s="4">
         <v>3</v>
@@ -1242,10 +1336,10 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>17</v>
@@ -1266,31 +1360,31 @@
         <v>17</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -1357,10 +1451,10 @@
     <row r="14" spans="1:23">
       <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1436,19 +1530,19 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1503,49 +1597,49 @@
     <row r="19" spans="1:23">
       <c r="A19" s="12"/>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -1634,10 +1728,10 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="12" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1688,7 +1782,7 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="10" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1716,51 +1810,55 @@
     <row r="27" spans="1:23">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="I27" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="S27" s="3"/>
       <c r="T27" s="13" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="U27" s="13"/>
       <c r="V27" s="13"/>
@@ -1778,14 +1876,12 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="H28" s="4">
         <v>3</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -1796,32 +1892,24 @@
         <f>SUM(C4:R4)</f>
         <v>82</v>
       </c>
-      <c r="S28" s="9"/>
-      <c r="T28" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
+      <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:23">
       <c r="A29" s="12"/>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -1830,7 +1918,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4">
         <f>SUM(C6:R6)</f>
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
@@ -1841,7 +1929,7 @@
     <row r="30" spans="1:23">
       <c r="A30" s="12"/>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1852,8 +1940,6 @@
         <v>3</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -1873,13 +1959,13 @@
     <row r="31" spans="1:23">
       <c r="A31" s="12"/>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C31" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D31" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E31" s="4">
         <v>18</v>
@@ -1890,8 +1976,6 @@
         <v>6</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -1903,10 +1987,12 @@
         <v>78</v>
       </c>
       <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
+      <c r="T31" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
     </row>
     <row r="32" spans="1:23">
       <c r="C32" s="4"/>
@@ -1916,8 +2002,6 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -1933,10 +2017,10 @@
     </row>
     <row r="33" spans="1:23">
       <c r="A33" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1945,10 +2029,14 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4">
-        <v>10</v>
-      </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -1968,7 +2056,7 @@
     <row r="34" spans="1:23">
       <c r="A34" s="12"/>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1979,8 +2067,6 @@
       <c r="I34" s="4">
         <v>2</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2005,8 +2091,6 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -2022,10 +2106,10 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" s="12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -2034,8 +2118,6 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -2055,7 +2137,7 @@
     <row r="37" spans="1:23">
       <c r="A37" s="12"/>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -2064,14 +2146,12 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="4">
-        <v>9</v>
-      </c>
-      <c r="K37" s="4">
-        <v>3</v>
-      </c>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="L37" s="4">
+        <v>9</v>
+      </c>
+      <c r="M37" s="4">
+        <v>3</v>
+      </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
@@ -2110,11 +2190,11 @@
       <c r="W38" s="4"/>
     </row>
     <row r="39" spans="1:23" ht="27">
-      <c r="A39" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>43</v>
+      <c r="A39" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -2154,9 +2234,342 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A26:W26"/>
-    <mergeCell ref="T28:W28"/>
+    <mergeCell ref="T31:W31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15">
+        <v>3</v>
+      </c>
+      <c r="H3" s="15">
+        <v>4</v>
+      </c>
+      <c r="I3" s="15">
+        <v>5</v>
+      </c>
+      <c r="J3" s="15">
+        <v>6</v>
+      </c>
+      <c r="K3" s="15">
+        <v>7</v>
+      </c>
+      <c r="L3" s="15">
+        <v>8</v>
+      </c>
+      <c r="M3" s="15">
+        <v>9</v>
+      </c>
+      <c r="N3" s="15">
+        <v>10</v>
+      </c>
+      <c r="O3" s="15">
+        <v>11</v>
+      </c>
+      <c r="P3" s="15">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>13</v>
+      </c>
+      <c r="R3" s="15">
+        <v>14</v>
+      </c>
+      <c r="S3" s="15">
+        <v>15</v>
+      </c>
+      <c r="T3" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="V4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E4:T4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>